<commit_message>
added 2025 all, updated q3 and q4
</commit_message>
<xml_diff>
--- a/data/2025_data/2025Q3.xlsx
+++ b/data/2025_data/2025Q3.xlsx
@@ -18,14 +18,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId12" roundtripDataChecksum="tFBZz1d7cNloEjVi9I69+Frc5CPYMxsq6Ehluxrl2do="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId12" roundtripDataChecksum="sMJHSj7wkJvJpN2+l1PsGgbcd+7uhgmpEHkRZH09hDM="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="217">
   <si>
     <t>date of publication</t>
   </si>
@@ -456,6 +456,30 @@
     <t>2</t>
   </si>
   <si>
+    <t>24.09.2025</t>
+  </si>
+  <si>
+    <t>Gender Equality and Its Significance for Scientific Research and Innovation</t>
+  </si>
+  <si>
+    <t>https://www.cogitatiopress.com/socialinclusion/article/viewFile/10105/4675</t>
+  </si>
+  <si>
+    <t>Cinzia Leone; Lina Donnarumma, Vanessa de Luca</t>
+  </si>
+  <si>
+    <t>Italian Institute of Technology</t>
+  </si>
+  <si>
+    <t>Social Inclusion Vol. 13</t>
+  </si>
+  <si>
+    <t>Gender Equality Plan</t>
+  </si>
+  <si>
+    <t>Promoting gender equality and women’s empowerment across the world</t>
+  </si>
+  <si>
     <t>31.08.2025</t>
   </si>
   <si>
@@ -529,9 +553,6 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Promoting gender equality and women’s empowerment across the world</t>
   </si>
   <si>
     <t>Methodological report</t>
@@ -807,7 +828,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="48">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -899,6 +920,18 @@
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="14" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="0"/>
     </xf>
@@ -908,9 +941,6 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="top"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="0"/>
@@ -2107,100 +2137,98 @@
       <c r="Z16" s="26"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="C17" s="31" t="s">
+      <c r="C17" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" s="32" t="s">
         <v>137</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F17" s="33" t="s">
         <v>138</v>
       </c>
-      <c r="G17" s="32"/>
-      <c r="H17" s="32"/>
-      <c r="I17" s="33"/>
-      <c r="J17" s="28"/>
-      <c r="K17" s="18"/>
-      <c r="L17" s="18"/>
-      <c r="M17" s="18"/>
-      <c r="N17" s="18"/>
-      <c r="O17" s="18"/>
-      <c r="P17" s="4">
-        <f t="shared" ref="P17:P19" si="3">L17*0.4+M17*0.1+N17*0.1</f>
-        <v>0</v>
-      </c>
-      <c r="Q17" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="R17" s="3"/>
-      <c r="S17" s="3"/>
-      <c r="T17" s="3"/>
-      <c r="U17" s="3"/>
-      <c r="V17" s="3"/>
-      <c r="W17" s="3"/>
-      <c r="X17" s="3"/>
-      <c r="Y17" s="3"/>
-      <c r="Z17" s="3"/>
+      <c r="G17" s="34" t="s">
+        <v>139</v>
+      </c>
+      <c r="H17" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="I17" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="J17" s="34" t="s">
+        <v>140</v>
+      </c>
+      <c r="K17" s="34">
+        <v>1.0</v>
+      </c>
+      <c r="L17" s="34">
+        <v>3.0</v>
+      </c>
+      <c r="M17" s="34">
+        <v>3.0</v>
+      </c>
+      <c r="N17" s="34">
+        <v>1.0</v>
+      </c>
+      <c r="O17" s="11"/>
+      <c r="P17" s="34">
+        <f>L17*0.4 + K17*0.2 + M17*0.1 + N17*0.1 + O17*0.2</f>
+        <v>1.8</v>
+      </c>
+      <c r="Q17" s="12"/>
+      <c r="R17" s="12"/>
+      <c r="S17" s="12"/>
+      <c r="T17" s="12"/>
+      <c r="U17" s="12"/>
+      <c r="V17" s="12"/>
+      <c r="W17" s="12"/>
+      <c r="X17" s="12"/>
+      <c r="Y17" s="12"/>
+      <c r="Z17" s="12"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="4" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>140</v>
+        <v>142</v>
+      </c>
+      <c r="C18" s="35" t="s">
+        <v>143</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="I18" s="4">
-        <v>2021.0</v>
-      </c>
-      <c r="J18" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="K18" s="4"/>
-      <c r="L18" s="4">
-        <v>4.0</v>
-      </c>
-      <c r="M18" s="4">
-        <v>2.0</v>
-      </c>
-      <c r="N18" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="O18" s="4">
-        <v>0.0</v>
-      </c>
+        <v>146</v>
+      </c>
+      <c r="G18" s="36"/>
+      <c r="H18" s="36"/>
+      <c r="I18" s="37"/>
+      <c r="J18" s="28"/>
+      <c r="K18" s="18"/>
+      <c r="L18" s="18"/>
+      <c r="M18" s="18"/>
+      <c r="N18" s="18"/>
+      <c r="O18" s="18"/>
       <c r="P18" s="4">
-        <f t="shared" si="3"/>
-        <v>1.9</v>
+        <f t="shared" ref="P18:P20" si="3">L18*0.4+M18*0.1+N18*0.1</f>
+        <v>0</v>
       </c>
       <c r="Q18" s="4" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="R18" s="3"/>
       <c r="S18" s="3"/>
@@ -2214,38 +2242,38 @@
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="4" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="E19" s="34" t="s">
-        <v>148</v>
-      </c>
-      <c r="F19" s="26" t="s">
         <v>149</v>
       </c>
+      <c r="E19" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="G19" s="3" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="I19" s="4" t="s">
-        <v>25</v>
+        <v>34</v>
+      </c>
+      <c r="I19" s="4">
+        <v>2021.0</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>26</v>
+        <v>93</v>
       </c>
       <c r="K19" s="4"/>
       <c r="L19" s="4">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="M19" s="4">
         <v>2.0</v>
@@ -2253,12 +2281,12 @@
       <c r="N19" s="4">
         <v>1.0</v>
       </c>
-      <c r="O19" s="6">
+      <c r="O19" s="4">
         <v>0.0</v>
       </c>
       <c r="P19" s="4">
         <f t="shared" si="3"/>
-        <v>1.1</v>
+        <v>1.9</v>
       </c>
       <c r="Q19" s="4" t="s">
         <v>45</v>
@@ -2274,93 +2302,126 @@
       <c r="Z19" s="3"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="29" t="s">
-        <v>133</v>
-      </c>
-      <c r="B20" s="35" t="s">
-        <v>151</v>
+      <c r="A20" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>153</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="D20" s="35" t="s">
-        <v>153</v>
-      </c>
-      <c r="E20" s="35" t="s">
         <v>154</v>
       </c>
-      <c r="F20" s="35" t="s">
+      <c r="D20" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="G20" s="35" t="s">
+      <c r="E20" s="38" t="s">
         <v>156</v>
       </c>
-      <c r="H20" s="35" t="s">
+      <c r="F20" s="26" t="s">
+        <v>157</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="M20" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="N20" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="O20" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="P20" s="4">
+        <f t="shared" si="3"/>
+        <v>1.1</v>
+      </c>
+      <c r="Q20" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="R20" s="3"/>
+      <c r="S20" s="3"/>
+      <c r="T20" s="3"/>
+      <c r="U20" s="3"/>
+      <c r="V20" s="3"/>
+      <c r="W20" s="3"/>
+      <c r="X20" s="3"/>
+      <c r="Y20" s="3"/>
+      <c r="Z20" s="3"/>
+    </row>
+    <row r="21" ht="15.75" customHeight="1">
+      <c r="A21" s="29" t="s">
+        <v>141</v>
+      </c>
+      <c r="B21" s="33" t="s">
+        <v>159</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="D21" s="33" t="s">
+        <v>161</v>
+      </c>
+      <c r="E21" s="33" t="s">
+        <v>162</v>
+      </c>
+      <c r="F21" s="33" t="s">
+        <v>163</v>
+      </c>
+      <c r="G21" s="33" t="s">
+        <v>164</v>
+      </c>
+      <c r="H21" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="I20" s="35">
+      <c r="I21" s="33">
         <v>2025.0</v>
       </c>
-      <c r="J20" s="35" t="s">
+      <c r="J21" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="K20" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="L20" s="35">
+      <c r="K21" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="L21" s="33">
         <v>2.0</v>
       </c>
-      <c r="M20" s="35">
+      <c r="M21" s="33">
         <v>2.0</v>
       </c>
-      <c r="N20" s="35">
+      <c r="N21" s="33">
         <v>1.0</v>
       </c>
-      <c r="O20" s="11"/>
-      <c r="P20" s="26"/>
-      <c r="Q20" s="26"/>
-      <c r="R20" s="26"/>
-      <c r="S20" s="26"/>
-      <c r="T20" s="26"/>
-      <c r="U20" s="26"/>
-      <c r="V20" s="26"/>
-      <c r="W20" s="26"/>
-      <c r="X20" s="26"/>
-      <c r="Y20" s="26"/>
-      <c r="Z20" s="26"/>
-    </row>
-    <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="4"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="36"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="4"/>
-      <c r="M21" s="4"/>
-      <c r="N21" s="4"/>
-      <c r="O21" s="4"/>
-      <c r="P21" s="4"/>
-      <c r="Q21" s="4"/>
-      <c r="R21" s="3"/>
-      <c r="S21" s="3"/>
-      <c r="T21" s="3"/>
-      <c r="U21" s="3"/>
-      <c r="V21" s="3"/>
-      <c r="W21" s="3"/>
-      <c r="X21" s="3"/>
-      <c r="Y21" s="3"/>
-      <c r="Z21" s="3"/>
+      <c r="O21" s="11"/>
+      <c r="P21" s="26"/>
+      <c r="Q21" s="26"/>
+      <c r="R21" s="26"/>
+      <c r="S21" s="26"/>
+      <c r="T21" s="26"/>
+      <c r="U21" s="26"/>
+      <c r="V21" s="26"/>
+      <c r="W21" s="26"/>
+      <c r="X21" s="26"/>
+      <c r="Y21" s="26"/>
+      <c r="Z21" s="26"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="4"/>
       <c r="B22" s="3"/>
-      <c r="C22" s="5"/>
+      <c r="C22" s="39"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
@@ -28986,183 +29047,211 @@
       <c r="Z972" s="3"/>
     </row>
     <row r="973" ht="15.75" customHeight="1">
-      <c r="A973" s="37"/>
-      <c r="C973" s="38"/>
-      <c r="I973" s="37"/>
-      <c r="K973" s="37"/>
-      <c r="L973" s="37"/>
-      <c r="M973" s="37"/>
-      <c r="N973" s="37"/>
-      <c r="O973" s="37"/>
-      <c r="P973" s="37"/>
-      <c r="Q973" s="37"/>
+      <c r="A973" s="4"/>
+      <c r="B973" s="3"/>
+      <c r="C973" s="5"/>
+      <c r="D973" s="3"/>
+      <c r="E973" s="3"/>
+      <c r="F973" s="3"/>
+      <c r="G973" s="3"/>
+      <c r="H973" s="3"/>
+      <c r="I973" s="4"/>
+      <c r="J973" s="3"/>
+      <c r="K973" s="4"/>
+      <c r="L973" s="4"/>
+      <c r="M973" s="4"/>
+      <c r="N973" s="4"/>
+      <c r="O973" s="4"/>
+      <c r="P973" s="4"/>
+      <c r="Q973" s="4"/>
+      <c r="R973" s="3"/>
+      <c r="S973" s="3"/>
+      <c r="T973" s="3"/>
+      <c r="U973" s="3"/>
+      <c r="V973" s="3"/>
+      <c r="W973" s="3"/>
+      <c r="X973" s="3"/>
+      <c r="Y973" s="3"/>
+      <c r="Z973" s="3"/>
     </row>
     <row r="974" ht="15.75" customHeight="1">
-      <c r="A974" s="37"/>
-      <c r="C974" s="38"/>
-      <c r="I974" s="37"/>
-      <c r="K974" s="37"/>
-      <c r="L974" s="37"/>
-      <c r="M974" s="37"/>
-      <c r="N974" s="37"/>
-      <c r="O974" s="37"/>
-      <c r="P974" s="37"/>
-      <c r="Q974" s="37"/>
+      <c r="A974" s="40"/>
+      <c r="C974" s="41"/>
+      <c r="I974" s="40"/>
+      <c r="K974" s="40"/>
+      <c r="L974" s="40"/>
+      <c r="M974" s="40"/>
+      <c r="N974" s="40"/>
+      <c r="O974" s="40"/>
+      <c r="P974" s="40"/>
+      <c r="Q974" s="40"/>
     </row>
     <row r="975" ht="15.75" customHeight="1">
-      <c r="A975" s="37"/>
-      <c r="C975" s="38"/>
-      <c r="I975" s="37"/>
-      <c r="K975" s="37"/>
-      <c r="L975" s="37"/>
-      <c r="M975" s="37"/>
-      <c r="N975" s="37"/>
-      <c r="O975" s="37"/>
-      <c r="P975" s="37"/>
-      <c r="Q975" s="37"/>
+      <c r="A975" s="40"/>
+      <c r="C975" s="41"/>
+      <c r="I975" s="40"/>
+      <c r="K975" s="40"/>
+      <c r="L975" s="40"/>
+      <c r="M975" s="40"/>
+      <c r="N975" s="40"/>
+      <c r="O975" s="40"/>
+      <c r="P975" s="40"/>
+      <c r="Q975" s="40"/>
     </row>
     <row r="976" ht="15.75" customHeight="1">
-      <c r="A976" s="37"/>
-      <c r="C976" s="38"/>
-      <c r="I976" s="37"/>
-      <c r="K976" s="37"/>
-      <c r="L976" s="37"/>
-      <c r="M976" s="37"/>
-      <c r="N976" s="37"/>
-      <c r="O976" s="37"/>
-      <c r="P976" s="37"/>
-      <c r="Q976" s="37"/>
+      <c r="A976" s="40"/>
+      <c r="C976" s="41"/>
+      <c r="I976" s="40"/>
+      <c r="K976" s="40"/>
+      <c r="L976" s="40"/>
+      <c r="M976" s="40"/>
+      <c r="N976" s="40"/>
+      <c r="O976" s="40"/>
+      <c r="P976" s="40"/>
+      <c r="Q976" s="40"/>
     </row>
     <row r="977" ht="15.75" customHeight="1">
-      <c r="A977" s="37"/>
-      <c r="C977" s="38"/>
-      <c r="I977" s="37"/>
-      <c r="K977" s="37"/>
-      <c r="L977" s="37"/>
-      <c r="M977" s="37"/>
-      <c r="N977" s="37"/>
-      <c r="O977" s="37"/>
-      <c r="P977" s="37"/>
-      <c r="Q977" s="37"/>
+      <c r="A977" s="40"/>
+      <c r="C977" s="41"/>
+      <c r="I977" s="40"/>
+      <c r="K977" s="40"/>
+      <c r="L977" s="40"/>
+      <c r="M977" s="40"/>
+      <c r="N977" s="40"/>
+      <c r="O977" s="40"/>
+      <c r="P977" s="40"/>
+      <c r="Q977" s="40"/>
     </row>
     <row r="978" ht="15.75" customHeight="1">
-      <c r="A978" s="37"/>
-      <c r="C978" s="38"/>
-      <c r="I978" s="37"/>
-      <c r="K978" s="37"/>
-      <c r="L978" s="37"/>
-      <c r="M978" s="37"/>
-      <c r="N978" s="37"/>
-      <c r="O978" s="37"/>
-      <c r="P978" s="37"/>
-      <c r="Q978" s="37"/>
+      <c r="A978" s="40"/>
+      <c r="C978" s="41"/>
+      <c r="I978" s="40"/>
+      <c r="K978" s="40"/>
+      <c r="L978" s="40"/>
+      <c r="M978" s="40"/>
+      <c r="N978" s="40"/>
+      <c r="O978" s="40"/>
+      <c r="P978" s="40"/>
+      <c r="Q978" s="40"/>
     </row>
     <row r="979" ht="15.75" customHeight="1">
-      <c r="A979" s="37"/>
-      <c r="C979" s="38"/>
-      <c r="I979" s="37"/>
-      <c r="K979" s="37"/>
-      <c r="L979" s="37"/>
-      <c r="M979" s="37"/>
-      <c r="N979" s="37"/>
-      <c r="O979" s="37"/>
-      <c r="P979" s="37"/>
-      <c r="Q979" s="37"/>
+      <c r="A979" s="40"/>
+      <c r="C979" s="41"/>
+      <c r="I979" s="40"/>
+      <c r="K979" s="40"/>
+      <c r="L979" s="40"/>
+      <c r="M979" s="40"/>
+      <c r="N979" s="40"/>
+      <c r="O979" s="40"/>
+      <c r="P979" s="40"/>
+      <c r="Q979" s="40"/>
     </row>
     <row r="980" ht="15.75" customHeight="1">
-      <c r="A980" s="37"/>
-      <c r="C980" s="38"/>
-      <c r="I980" s="37"/>
-      <c r="K980" s="37"/>
-      <c r="L980" s="37"/>
-      <c r="M980" s="37"/>
-      <c r="N980" s="37"/>
-      <c r="O980" s="37"/>
-      <c r="P980" s="37"/>
-      <c r="Q980" s="37"/>
+      <c r="A980" s="40"/>
+      <c r="C980" s="41"/>
+      <c r="I980" s="40"/>
+      <c r="K980" s="40"/>
+      <c r="L980" s="40"/>
+      <c r="M980" s="40"/>
+      <c r="N980" s="40"/>
+      <c r="O980" s="40"/>
+      <c r="P980" s="40"/>
+      <c r="Q980" s="40"/>
     </row>
     <row r="981" ht="15.75" customHeight="1">
-      <c r="A981" s="37"/>
-      <c r="C981" s="38"/>
-      <c r="I981" s="37"/>
-      <c r="K981" s="37"/>
-      <c r="L981" s="37"/>
-      <c r="M981" s="37"/>
-      <c r="N981" s="37"/>
-      <c r="O981" s="37"/>
-      <c r="P981" s="37"/>
-      <c r="Q981" s="37"/>
+      <c r="A981" s="40"/>
+      <c r="C981" s="41"/>
+      <c r="I981" s="40"/>
+      <c r="K981" s="40"/>
+      <c r="L981" s="40"/>
+      <c r="M981" s="40"/>
+      <c r="N981" s="40"/>
+      <c r="O981" s="40"/>
+      <c r="P981" s="40"/>
+      <c r="Q981" s="40"/>
     </row>
     <row r="982" ht="15.75" customHeight="1">
-      <c r="A982" s="37"/>
-      <c r="C982" s="38"/>
-      <c r="I982" s="37"/>
-      <c r="K982" s="37"/>
-      <c r="L982" s="37"/>
-      <c r="M982" s="37"/>
-      <c r="N982" s="37"/>
-      <c r="O982" s="37"/>
-      <c r="P982" s="37"/>
-      <c r="Q982" s="37"/>
+      <c r="A982" s="40"/>
+      <c r="C982" s="41"/>
+      <c r="I982" s="40"/>
+      <c r="K982" s="40"/>
+      <c r="L982" s="40"/>
+      <c r="M982" s="40"/>
+      <c r="N982" s="40"/>
+      <c r="O982" s="40"/>
+      <c r="P982" s="40"/>
+      <c r="Q982" s="40"/>
     </row>
     <row r="983" ht="15.75" customHeight="1">
-      <c r="A983" s="37"/>
-      <c r="C983" s="38"/>
-      <c r="I983" s="37"/>
-      <c r="K983" s="37"/>
-      <c r="L983" s="37"/>
-      <c r="M983" s="37"/>
-      <c r="N983" s="37"/>
-      <c r="O983" s="37"/>
-      <c r="P983" s="37"/>
-      <c r="Q983" s="37"/>
+      <c r="A983" s="40"/>
+      <c r="C983" s="41"/>
+      <c r="I983" s="40"/>
+      <c r="K983" s="40"/>
+      <c r="L983" s="40"/>
+      <c r="M983" s="40"/>
+      <c r="N983" s="40"/>
+      <c r="O983" s="40"/>
+      <c r="P983" s="40"/>
+      <c r="Q983" s="40"/>
     </row>
     <row r="984" ht="15.75" customHeight="1">
-      <c r="A984" s="37"/>
-      <c r="C984" s="38"/>
-      <c r="I984" s="37"/>
-      <c r="K984" s="37"/>
-      <c r="L984" s="37"/>
-      <c r="M984" s="37"/>
-      <c r="N984" s="37"/>
-      <c r="O984" s="37"/>
-      <c r="P984" s="37"/>
-      <c r="Q984" s="37"/>
+      <c r="A984" s="40"/>
+      <c r="C984" s="41"/>
+      <c r="I984" s="40"/>
+      <c r="K984" s="40"/>
+      <c r="L984" s="40"/>
+      <c r="M984" s="40"/>
+      <c r="N984" s="40"/>
+      <c r="O984" s="40"/>
+      <c r="P984" s="40"/>
+      <c r="Q984" s="40"/>
     </row>
     <row r="985" ht="15.75" customHeight="1">
-      <c r="A985" s="37"/>
-      <c r="C985" s="38"/>
-      <c r="I985" s="37"/>
-      <c r="K985" s="37"/>
-      <c r="L985" s="37"/>
-      <c r="M985" s="37"/>
-      <c r="N985" s="37"/>
-      <c r="O985" s="37"/>
-      <c r="P985" s="37"/>
-      <c r="Q985" s="37"/>
+      <c r="A985" s="40"/>
+      <c r="C985" s="41"/>
+      <c r="I985" s="40"/>
+      <c r="K985" s="40"/>
+      <c r="L985" s="40"/>
+      <c r="M985" s="40"/>
+      <c r="N985" s="40"/>
+      <c r="O985" s="40"/>
+      <c r="P985" s="40"/>
+      <c r="Q985" s="40"/>
+    </row>
+    <row r="986" ht="15.75" customHeight="1">
+      <c r="A986" s="40"/>
+      <c r="C986" s="41"/>
+      <c r="I986" s="40"/>
+      <c r="K986" s="40"/>
+      <c r="L986" s="40"/>
+      <c r="M986" s="40"/>
+      <c r="N986" s="40"/>
+      <c r="O986" s="40"/>
+      <c r="P986" s="40"/>
+      <c r="Q986" s="40"/>
     </row>
   </sheetData>
   <autoFilter ref="$A$1:$Q$1"/>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="N1:N6 N8:N12 N14:N16 N18:N972">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="N1:N6 N8:N12 N14:N17 N19:N973">
       <formula1>'category of mention'!$A$1:$A$3</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H1:H6 H8:H16 H18:H972">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H1:H6 H8:H17 H19:H973">
       <formula1>'type of EIGE output'!$A$1:$A$13</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="K1:K6 K8:K12 K14:K16 K18:K972">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="K1:K6 K8:K12 K14:K17 K19:K973">
       <formula1>'impact factor'!$A$1:$A$3</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="M1:M6 M8:M12 M14:M16 M18:M972">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="M1:M6 M8:M12 M14:M17 M19:M973">
       <formula1>'location of the citation'!$A$1:$A$3</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="J1:J972">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="J1:J973">
       <formula1>topic!$A$1:$A$5</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="F10"/>
-    <hyperlink r:id="rId2" ref="E19"/>
+    <hyperlink r:id="rId2" ref="E20"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
@@ -29186,28 +29275,28 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="42" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="42" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="42" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="42" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="39" t="s">
-        <v>158</v>
+      <c r="A5" s="42" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1"/>
@@ -30227,73 +30316,73 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="43" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="40" t="s">
-        <v>159</v>
+      <c r="A2" s="43" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="43" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="40" t="s">
-        <v>160</v>
+      <c r="A4" s="43" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="43" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="43" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="40" t="s">
-        <v>161</v>
+      <c r="A7" s="43" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="40" t="s">
+      <c r="A8" s="43" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="40" t="s">
+      <c r="A9" s="43" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="40" t="s">
-        <v>162</v>
+      <c r="A10" s="43" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="40" t="s">
-        <v>163</v>
+      <c r="A11" s="43" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="40" t="s">
+      <c r="A12" s="43" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="40" t="s">
+      <c r="A13" s="43" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="40" t="s">
-        <v>164</v>
+      <c r="A14" s="43" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1"/>
@@ -31310,105 +31399,105 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="41" t="s">
-        <v>165</v>
-      </c>
-      <c r="B1" s="41" t="s">
-        <v>166</v>
-      </c>
-      <c r="C1" s="41" t="s">
-        <v>167</v>
-      </c>
-      <c r="D1" s="41" t="s">
-        <v>168</v>
-      </c>
-      <c r="E1" s="41" t="s">
-        <v>169</v>
+      <c r="A1" s="44" t="s">
+        <v>172</v>
+      </c>
+      <c r="B1" s="44" t="s">
+        <v>173</v>
+      </c>
+      <c r="C1" s="44" t="s">
+        <v>174</v>
+      </c>
+      <c r="D1" s="44" t="s">
+        <v>175</v>
+      </c>
+      <c r="E1" s="44" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="40" t="s">
-        <v>170</v>
-      </c>
-      <c r="B2" s="40" t="s">
+      <c r="A2" s="43" t="s">
+        <v>177</v>
+      </c>
+      <c r="B2" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="40" t="s">
-        <v>171</v>
-      </c>
-      <c r="D2" s="40" t="s">
-        <v>172</v>
-      </c>
-      <c r="E2" s="40" t="s">
-        <v>173</v>
+      <c r="C2" s="43" t="s">
+        <v>178</v>
+      </c>
+      <c r="D2" s="43" t="s">
+        <v>179</v>
+      </c>
+      <c r="E2" s="43" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="40" t="s">
-        <v>174</v>
-      </c>
-      <c r="B3" s="40" t="s">
-        <v>175</v>
-      </c>
-      <c r="C3" s="40" t="s">
-        <v>176</v>
-      </c>
-      <c r="D3" s="40" t="s">
-        <v>172</v>
-      </c>
-      <c r="E3" s="40" t="s">
-        <v>173</v>
+      <c r="A3" s="43" t="s">
+        <v>181</v>
+      </c>
+      <c r="B3" s="43" t="s">
+        <v>182</v>
+      </c>
+      <c r="C3" s="43" t="s">
+        <v>183</v>
+      </c>
+      <c r="D3" s="43" t="s">
+        <v>179</v>
+      </c>
+      <c r="E3" s="43" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="40" t="s">
-        <v>174</v>
-      </c>
-      <c r="B4" s="40" t="s">
-        <v>177</v>
-      </c>
-      <c r="C4" s="40" t="s">
-        <v>176</v>
-      </c>
-      <c r="D4" s="40" t="s">
-        <v>172</v>
-      </c>
-      <c r="E4" s="40" t="s">
-        <v>173</v>
+      <c r="A4" s="43" t="s">
+        <v>181</v>
+      </c>
+      <c r="B4" s="43" t="s">
+        <v>184</v>
+      </c>
+      <c r="C4" s="43" t="s">
+        <v>183</v>
+      </c>
+      <c r="D4" s="43" t="s">
+        <v>179</v>
+      </c>
+      <c r="E4" s="43" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="40" t="s">
-        <v>178</v>
-      </c>
-      <c r="B5" s="40" t="s">
+      <c r="A5" s="43" t="s">
+        <v>185</v>
+      </c>
+      <c r="B5" s="43" t="s">
+        <v>186</v>
+      </c>
+      <c r="C5" s="43" t="s">
+        <v>183</v>
+      </c>
+      <c r="D5" s="43" t="s">
         <v>179</v>
       </c>
-      <c r="C5" s="40" t="s">
-        <v>176</v>
-      </c>
-      <c r="D5" s="40" t="s">
-        <v>172</v>
-      </c>
-      <c r="E5" s="40" t="s">
-        <v>180</v>
+      <c r="E5" s="43" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="40" t="s">
-        <v>181</v>
-      </c>
-      <c r="B6" s="40" t="s">
-        <v>182</v>
-      </c>
-      <c r="C6" s="40" t="s">
-        <v>183</v>
-      </c>
-      <c r="D6" s="40" t="s">
-        <v>172</v>
-      </c>
-      <c r="E6" s="40" t="s">
-        <v>184</v>
+      <c r="A6" s="43" t="s">
+        <v>188</v>
+      </c>
+      <c r="B6" s="43" t="s">
+        <v>189</v>
+      </c>
+      <c r="C6" s="43" t="s">
+        <v>190</v>
+      </c>
+      <c r="D6" s="43" t="s">
+        <v>179</v>
+      </c>
+      <c r="E6" s="43" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1"/>
@@ -31419,8 +31508,8 @@
     <row r="12" ht="15.75" customHeight="1"/>
     <row r="13" ht="15.75" customHeight="1"/>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="40" t="s">
-        <v>185</v>
+      <c r="A14" s="43" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1"/>
@@ -31434,7 +31523,7 @@
     <row r="23" ht="15.75" customHeight="1"/>
     <row r="24" ht="15.75" customHeight="1"/>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="C25" s="37"/>
+      <c r="C25" s="40"/>
     </row>
     <row r="26" ht="15.75" customHeight="1"/>
     <row r="27" ht="15.75" customHeight="1"/>
@@ -32433,53 +32522,53 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="42" t="s">
-        <v>186</v>
-      </c>
-      <c r="B1" s="40" t="s">
-        <v>187</v>
-      </c>
-      <c r="C1" s="40" t="s">
-        <v>188</v>
-      </c>
-      <c r="D1" s="40" t="s">
-        <v>189</v>
+      <c r="A1" s="45" t="s">
+        <v>193</v>
+      </c>
+      <c r="B1" s="43" t="s">
+        <v>194</v>
+      </c>
+      <c r="C1" s="43" t="s">
+        <v>195</v>
+      </c>
+      <c r="D1" s="43" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="45" t="s">
         <v>132</v>
       </c>
-      <c r="B2" s="40" t="s">
-        <v>190</v>
-      </c>
-      <c r="C2" s="40" t="s">
-        <v>191</v>
-      </c>
-      <c r="D2" s="40" t="s">
-        <v>192</v>
+      <c r="B2" s="43" t="s">
+        <v>197</v>
+      </c>
+      <c r="C2" s="43" t="s">
+        <v>198</v>
+      </c>
+      <c r="D2" s="43" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="42" t="s">
-        <v>193</v>
-      </c>
-      <c r="B3" s="40" t="s">
-        <v>194</v>
-      </c>
-      <c r="C3" s="40" t="s">
-        <v>195</v>
-      </c>
-      <c r="D3" s="40" t="s">
-        <v>196</v>
+      <c r="A3" s="45" t="s">
+        <v>200</v>
+      </c>
+      <c r="B3" s="43" t="s">
+        <v>201</v>
+      </c>
+      <c r="C3" s="43" t="s">
+        <v>202</v>
+      </c>
+      <c r="D3" s="43" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="43">
+      <c r="A4" s="46">
         <v>0.0</v>
       </c>
-      <c r="B4" s="40" t="s">
-        <v>197</v>
+      <c r="B4" s="43" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1"/>
@@ -33500,27 +33589,27 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="40">
+      <c r="A1" s="43">
         <v>3.0</v>
       </c>
-      <c r="B1" s="40" t="s">
-        <v>198</v>
+      <c r="B1" s="43" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="40">
+      <c r="A2" s="43">
         <v>2.0</v>
       </c>
-      <c r="B2" s="40" t="s">
-        <v>199</v>
+      <c r="B2" s="43" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="40">
+      <c r="A3" s="43">
         <v>1.0</v>
       </c>
-      <c r="B3" s="40" t="s">
-        <v>200</v>
+      <c r="B3" s="43" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1"/>
@@ -34542,27 +34631,27 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="40">
+      <c r="A1" s="43">
         <v>1.0</v>
       </c>
-      <c r="B1" s="40" t="s">
-        <v>201</v>
+      <c r="B1" s="43" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="40">
+      <c r="A2" s="43">
         <v>0.0</v>
       </c>
-      <c r="B2" s="40" t="s">
-        <v>202</v>
+      <c r="B2" s="43" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="42" t="s">
-        <v>203</v>
-      </c>
-      <c r="B3" s="40" t="s">
-        <v>204</v>
+      <c r="A3" s="45" t="s">
+        <v>210</v>
+      </c>
+      <c r="B3" s="43" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1"/>
@@ -35585,50 +35674,50 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="44" t="s">
-        <v>205</v>
-      </c>
-      <c r="B1" s="44" t="s">
-        <v>206</v>
+      <c r="A1" s="47" t="s">
+        <v>212</v>
+      </c>
+      <c r="B1" s="47" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="2" ht="16.5" customHeight="1">
-      <c r="A2" s="40" t="s">
-        <v>207</v>
-      </c>
-      <c r="B2" s="40">
+      <c r="A2" s="43" t="s">
+        <v>214</v>
+      </c>
+      <c r="B2" s="43">
         <v>0.4</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="40" t="s">
-        <v>181</v>
-      </c>
-      <c r="B3" s="40">
+      <c r="A3" s="43" t="s">
+        <v>188</v>
+      </c>
+      <c r="B3" s="43">
         <v>0.2</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="40" t="s">
-        <v>179</v>
-      </c>
-      <c r="B4" s="40">
+      <c r="A4" s="43" t="s">
+        <v>186</v>
+      </c>
+      <c r="B4" s="43">
         <v>0.2</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="40" t="s">
-        <v>208</v>
-      </c>
-      <c r="B5" s="40">
+      <c r="A5" s="43" t="s">
+        <v>215</v>
+      </c>
+      <c r="B5" s="43">
         <v>0.1</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="40" t="s">
-        <v>209</v>
-      </c>
-      <c r="B6" s="40">
+      <c r="A6" s="43" t="s">
+        <v>216</v>
+      </c>
+      <c r="B6" s="43">
         <v>0.1</v>
       </c>
     </row>

</xml_diff>